<commit_message>
nova iteracio i primera jornada 16 17
</commit_message>
<xml_diff>
--- a/excelcalc.xlsx
+++ b/excelcalc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
   <si>
     <t>0 10,5 F</t>
   </si>
@@ -99,24 +99,15 @@
     <t>O9,5T</t>
   </si>
   <si>
-    <t>[AC Milan]</t>
-  </si>
-  <si>
     <t>[AFC Bournemouth]</t>
   </si>
   <si>
-    <t>[AS Roma]</t>
+    <t>[Alaves]</t>
   </si>
   <si>
     <t>[Arsenal]</t>
   </si>
   <si>
-    <t>[Aston Villa]</t>
-  </si>
-  <si>
-    <t>[Atalanta]</t>
-  </si>
-  <si>
     <t>[Athletic Bilbao]</t>
   </si>
   <si>
@@ -129,19 +120,13 @@
     <t>[Bayer Leverkusen]</t>
   </si>
   <si>
-    <t>[Bayern Munich]</t>
-  </si>
-  <si>
-    <t>[Bologna]</t>
-  </si>
-  <si>
     <t>[Borussia Dortmund]</t>
   </si>
   <si>
     <t>[Borussia Monchengladbach]</t>
   </si>
   <si>
-    <t>[Carpi]</t>
+    <t>[Burnley]</t>
   </si>
   <si>
     <t>[Celta Vigo]</t>
@@ -150,9 +135,6 @@
     <t>[Chelsea]</t>
   </si>
   <si>
-    <t>[Chievo Verona]</t>
-  </si>
-  <si>
     <t>[Crystal Palace]</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
     <t>[Eintracht Frankfurt]</t>
   </si>
   <si>
-    <t>[Empoli]</t>
-  </si>
-  <si>
     <t>[Espanyol]</t>
   </si>
   <si>
@@ -183,49 +162,28 @@
     <t>[FC Ingolstadt 04]</t>
   </si>
   <si>
-    <t>[Fiorentina]</t>
-  </si>
-  <si>
-    <t>[Frosinone]</t>
-  </si>
-  <si>
-    <t>[Genoa]</t>
-  </si>
-  <si>
-    <t>[Getafe]</t>
-  </si>
-  <si>
     <t>[Granada]</t>
   </si>
   <si>
     <t>[Hamburg SV]</t>
   </si>
   <si>
-    <t>[Hannover 96]</t>
-  </si>
-  <si>
-    <t>[Hellas Verona]</t>
-  </si>
-  <si>
     <t>[Hertha Berlin]</t>
   </si>
   <si>
-    <t>[Internazionale]</t>
-  </si>
-  <si>
-    <t>[Juventus]</t>
+    <t>[Hull City]</t>
   </si>
   <si>
     <t>[Las Palmas]</t>
   </si>
   <si>
-    <t>[Lazio]</t>
+    <t>[Leganes]</t>
   </si>
   <si>
     <t>[Leicester City]</t>
   </si>
   <si>
-    <t>[Levante]</t>
+    <t>[Liverpool]</t>
   </si>
   <si>
     <t>[Mainz]</t>
@@ -237,25 +195,13 @@
     <t>[Manchester United]</t>
   </si>
   <si>
+    <t>[Middlesbrough]</t>
+  </si>
+  <si>
     <t>[Málaga]</t>
   </si>
   <si>
-    <t>[Napoli]</t>
-  </si>
-  <si>
-    <t>[Newcastle United]</t>
-  </si>
-  <si>
-    <t>[Norwich City]</t>
-  </si>
-  <si>
-    <t>[Palermo]</t>
-  </si>
-  <si>
-    <t>[Rayo Vallecano]</t>
-  </si>
-  <si>
-    <t>[Real Betis]</t>
+    <t>[Osasuna]</t>
   </si>
   <si>
     <t>[Real Madrid]</t>
@@ -267,12 +213,6 @@
     <t>[SV Darmstadt 98]</t>
   </si>
   <si>
-    <t>[Sampdoria]</t>
-  </si>
-  <si>
-    <t>[Sassuolo]</t>
-  </si>
-  <si>
     <t>[Schalke 04]</t>
   </si>
   <si>
@@ -297,15 +237,9 @@
     <t>[TSG Hoffenheim]</t>
   </si>
   <si>
-    <t>[Torino]</t>
-  </si>
-  <si>
     <t>[Tottenham Hotspur]</t>
   </si>
   <si>
-    <t>[Udinese]</t>
-  </si>
-  <si>
     <t>[Valencia]</t>
   </si>
   <si>
@@ -322,6 +256,9 @@
   </si>
   <si>
     <t>[Werder Bremen]</t>
+  </si>
+  <si>
+    <t>[West Bromwich Albion]</t>
   </si>
   <si>
     <t>[West Ham United]</t>
@@ -897,93 +834,93 @@
     </row>
     <row spans="1:20" r="2">
       <c t="s" r="A2">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c t="s" r="B2">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c t="n" r="C2">
-        <v>63.33333333333333</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="D2">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="E2">
-        <v>53.333333333333336</v>
+        <v>85.71428571428571</v>
       </c>
       <c t="n" r="F2">
-        <v>63.33333333333333</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="G2">
-        <v>53.333333333333336</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="H2">
-        <v>50.0</v>
+        <v>71.42857142857143</v>
       </c>
       <c t="n" r="I2">
-        <v>66.66666666666666</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="J2">
-        <v>63.33333333333333</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="K2">
-        <v>60.0</v>
+        <v>85.71428571428571</v>
       </c>
       <c t="n" r="L2">
         <v>45</v>
       </c>
       <c t="n" r="M2">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c t="n" r="N2">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c t="n" r="O2">
-        <v>56.666666666666664</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="P2">
-        <v>53.333333333333336</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="Q2">
-        <v>60.0</v>
+        <v>57.14285714285714</v>
       </c>
       <c t="n" r="R2">
-        <v>50.0</v>
+        <v>33.33333333333333</v>
       </c>
       <c t="n" r="S2">
-        <v>43.333333333333336</v>
+        <v>33.33333333333333</v>
       </c>
       <c t="n" r="T2">
-        <v>50.0</v>
+        <v>57.14285714285714</v>
       </c>
     </row>
     <row spans="1:20" r="3">
       <c t="s" r="A3">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c t="s" r="B3">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c t="n" r="C3">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="D3">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="E3">
+        <v>73.33333333333333</v>
+      </c>
+      <c t="n" r="F3">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="G3">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="H3">
         <v>70.0</v>
       </c>
-      <c t="n" r="F3">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="G3">
-        <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="H3">
-        <v>63.33333333333333</v>
-      </c>
       <c t="n" r="I3">
-        <v>56.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="J3">
         <v>63.33333333333333</v>
@@ -992,1383 +929,1383 @@
         <v>76.66666666666667</v>
       </c>
       <c t="n" r="L3">
+        <v>38</v>
+      </c>
+      <c t="n" r="M3">
+        <v>73</v>
+      </c>
+      <c t="n" r="N3">
         <v>37</v>
       </c>
-      <c t="n" r="M3">
-        <v>79</v>
-      </c>
-      <c t="n" r="N3">
-        <v>43</v>
-      </c>
       <c t="n" r="O3">
         <v>53.333333333333336</v>
       </c>
       <c t="n" r="P3">
-        <v>73.33333333333333</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="Q3">
-        <v>66.66666666666666</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="R3">
         <v>50.0</v>
       </c>
       <c t="n" r="S3">
-        <v>60.0</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="T3">
-        <v>50.0</v>
+        <v>43.333333333333336</v>
       </c>
     </row>
     <row spans="1:20" r="4">
       <c t="s" r="A4">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c t="s" r="B4">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c t="n" r="C4">
         <v>53.333333333333336</v>
       </c>
       <c t="n" r="D4">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="E4">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="F4">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="G4">
+        <v>36.666666666666664</v>
+      </c>
+      <c t="n" r="H4">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="I4">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="J4">
         <v>46.666666666666664</v>
       </c>
-      <c t="n" r="E4">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="F4">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="G4">
+      <c t="n" r="K4">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="L4">
+        <v>43</v>
+      </c>
+      <c t="n" r="M4">
+        <v>87</v>
+      </c>
+      <c t="n" r="N4">
+        <v>47</v>
+      </c>
+      <c t="n" r="O4">
         <v>43.333333333333336</v>
       </c>
-      <c t="n" r="H4">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="I4">
-        <v>60.0</v>
-      </c>
-      <c t="n" r="J4">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="K4">
-        <v>60.0</v>
-      </c>
-      <c t="n" r="L4">
-        <v>42</v>
-      </c>
-      <c t="n" r="M4">
-        <v>83</v>
-      </c>
-      <c t="n" r="N4">
-        <v>43</v>
-      </c>
-      <c t="n" r="O4">
-        <v>40.0</v>
-      </c>
       <c t="n" r="P4">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="Q4">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="R4">
         <v>36.666666666666664</v>
       </c>
-      <c t="n" r="Q4">
-        <v>33.33333333333333</v>
-      </c>
-      <c t="n" r="R4">
-        <v>33.33333333333333</v>
-      </c>
       <c t="n" r="S4">
-        <v>30.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="T4">
-        <v>30.0</v>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row spans="1:20" r="5">
       <c t="s" r="A5">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c t="s" r="B5">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c t="n" r="C5">
+        <v>50.0</v>
+      </c>
+      <c t="n" r="D5">
+        <v>43.333333333333336</v>
+      </c>
+      <c t="n" r="E5">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="F5">
         <v>46.666666666666664</v>
       </c>
-      <c t="n" r="D5">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="E5">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="F5">
+      <c t="n" r="G5">
         <v>40.0</v>
-      </c>
-      <c t="n" r="G5">
-        <v>50.0</v>
       </c>
       <c t="n" r="H5">
         <v>50.0</v>
       </c>
       <c t="n" r="I5">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="J5">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="K5">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="L5">
+        <v>45</v>
+      </c>
+      <c t="n" r="M5">
+        <v>89</v>
+      </c>
+      <c t="n" r="N5">
+        <v>47</v>
+      </c>
+      <c t="n" r="O5">
+        <v>73.33333333333333</v>
+      </c>
+      <c t="n" r="P5">
+        <v>70.0</v>
+      </c>
+      <c t="n" r="Q5">
         <v>50.0</v>
       </c>
-      <c t="n" r="J5">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="K5">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="L5">
-        <v>44</v>
-      </c>
-      <c t="n" r="M5">
-        <v>85</v>
-      </c>
-      <c t="n" r="N5">
-        <v>43</v>
-      </c>
-      <c t="n" r="O5">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="P5">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="Q5">
-        <v>70.0</v>
-      </c>
       <c t="n" r="R5">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="S5">
         <v>43.333333333333336</v>
       </c>
-      <c t="n" r="S5">
-        <v>63.33333333333333</v>
-      </c>
       <c t="n" r="T5">
-        <v>53.333333333333336</v>
+        <v>30.0</v>
       </c>
     </row>
     <row spans="1:20" r="6">
       <c t="s" r="A6">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c t="s" r="B6">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c t="n" r="C6">
-        <v>60.0</v>
+        <v>57.89473684210527</v>
       </c>
       <c t="n" r="D6">
-        <v>66.66666666666666</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="E6">
-        <v>70.0</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="F6">
-        <v>56.666666666666664</v>
+        <v>52.63157894736842</v>
       </c>
       <c t="n" r="G6">
-        <v>60.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="H6">
-        <v>63.33333333333333</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="I6">
-        <v>63.33333333333333</v>
+        <v>68.42105263157895</v>
       </c>
       <c t="n" r="J6">
-        <v>66.66666666666666</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="K6">
         <v>70.0</v>
       </c>
       <c t="n" r="L6">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c t="n" r="M6">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c t="n" r="N6">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c t="n" r="O6">
-        <v>56.666666666666664</v>
+        <v>36.84210526315789</v>
       </c>
       <c t="n" r="P6">
-        <v>50.0</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="Q6">
-        <v>46.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="R6">
-        <v>53.333333333333336</v>
+        <v>31.57894736842105</v>
       </c>
       <c t="n" r="S6">
+        <v>30.0</v>
+      </c>
+      <c t="n" r="T6">
         <v>43.333333333333336</v>
-      </c>
-      <c t="n" r="T6">
-        <v>23.333333333333332</v>
       </c>
     </row>
     <row spans="1:20" r="7">
       <c t="s" r="A7">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c t="s" r="B7">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c t="n" r="C7">
-        <v>53.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="D7">
-        <v>53.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="E7">
+        <v>70.0</v>
+      </c>
+      <c t="n" r="F7">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="G7">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="H7">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="I7">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="J7">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="K7">
+        <v>76.66666666666667</v>
+      </c>
+      <c t="n" r="L7">
+        <v>47</v>
+      </c>
+      <c t="n" r="M7">
+        <v>88</v>
+      </c>
+      <c t="n" r="N7">
+        <v>44</v>
+      </c>
+      <c t="n" r="O7">
+        <v>80.0</v>
+      </c>
+      <c t="n" r="P7">
+        <v>80.0</v>
+      </c>
+      <c t="n" r="Q7">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="R7">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="S7">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="T7">
         <v>50.0</v>
-      </c>
-      <c t="n" r="F7">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="G7">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="H7">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="I7">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="J7">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="K7">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="L7">
-        <v>44</v>
-      </c>
-      <c t="n" r="M7">
-        <v>62</v>
-      </c>
-      <c t="n" r="N7">
-        <v>18</v>
-      </c>
-      <c t="n" r="O7">
-        <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="P7">
-        <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="Q7">
-        <v>44.44444444444444</v>
-      </c>
-      <c t="n" r="R7">
-        <v>33.33333333333333</v>
-      </c>
-      <c t="n" r="S7">
-        <v>33.33333333333333</v>
-      </c>
-      <c t="n" r="T7">
-        <v>33.33333333333333</v>
       </c>
     </row>
     <row spans="1:20" r="8">
       <c t="s" r="A8">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c t="s" r="B8">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c t="n" r="C8">
-        <v>61.111111111111114</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="D8">
-        <v>50.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="E8">
-        <v>56.666666666666664</v>
+        <v>nan</v>
       </c>
       <c t="n" r="F8">
-        <v>55.55555555555556</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="G8">
-        <v>43.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="H8">
-        <v>53.333333333333336</v>
+        <v>nan</v>
       </c>
       <c t="n" r="I8">
-        <v>72.22222222222221</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="J8">
-        <v>60.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="K8">
-        <v>63.33333333333333</v>
+        <v>nan</v>
       </c>
       <c t="n" r="L8">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c t="n" r="M8">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c t="n" r="N8">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c t="n" r="O8">
-        <v>38.88888888888889</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="P8">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="Q8">
-        <v>66.66666666666666</v>
+        <v>nan</v>
       </c>
       <c t="n" r="R8">
-        <v>33.33333333333333</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="S8">
-        <v>43.333333333333336</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="T8">
-        <v>53.333333333333336</v>
+        <v>nan</v>
       </c>
     </row>
     <row spans="1:20" r="9">
       <c t="s" r="A9">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c t="s" r="B9">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c t="n" r="C9">
-        <v>68.0</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="D9">
         <v>73.33333333333333</v>
       </c>
       <c t="n" r="E9">
+        <v>nan</v>
+      </c>
+      <c t="n" r="F9">
         <v>70.0</v>
       </c>
-      <c t="n" r="F9">
-        <v>60.0</v>
-      </c>
       <c t="n" r="G9">
-        <v>66.66666666666666</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="H9">
-        <v>63.33333333333333</v>
+        <v>nan</v>
       </c>
       <c t="n" r="I9">
-        <v>76.0</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="J9">
         <v>73.33333333333333</v>
       </c>
       <c t="n" r="K9">
-        <v>73.33333333333333</v>
+        <v>nan</v>
       </c>
       <c t="n" r="L9">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c t="n" r="M9">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c t="n" r="N9">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c t="n" r="O9">
-        <v>52.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="P9">
-        <v>50.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="Q9">
-        <v>56.666666666666664</v>
+        <v>nan</v>
       </c>
       <c t="n" r="R9">
         <v>40.0</v>
       </c>
       <c t="n" r="S9">
-        <v>33.33333333333333</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="T9">
-        <v>46.666666666666664</v>
+        <v>nan</v>
       </c>
     </row>
     <row spans="1:20" r="10">
       <c t="s" r="A10">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c t="s" r="B10">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c t="n" r="C10">
-        <v>76.66666666666667</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="D10">
-        <v>66.66666666666666</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="E10">
-        <v>60.0</v>
+        <v>52.63157894736842</v>
       </c>
       <c t="n" r="F10">
-        <v>70.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="G10">
-        <v>66.66666666666666</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="H10">
-        <v>60.0</v>
+        <v>52.63157894736842</v>
       </c>
       <c t="n" r="I10">
-        <v>80.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="J10">
-        <v>70.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="K10">
-        <v>63.33333333333333</v>
+        <v>52.63157894736842</v>
       </c>
       <c t="n" r="L10">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c t="n" r="M10">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c t="n" r="N10">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c t="n" r="O10">
-        <v>53.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="P10">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="Q10">
-        <v>46.666666666666664</v>
+        <v>42.10526315789473</v>
       </c>
       <c t="n" r="R10">
+        <v>50.0</v>
+      </c>
+      <c t="n" r="S10">
         <v>43.333333333333336</v>
       </c>
-      <c t="n" r="S10">
-        <v>40.0</v>
-      </c>
       <c t="n" r="T10">
-        <v>33.33333333333333</v>
+        <v>31.57894736842105</v>
       </c>
     </row>
     <row spans="1:20" r="11">
       <c t="s" r="A11">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c t="s" r="B11">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c t="n" r="C11">
-        <v>56.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="D11">
         <v>46.666666666666664</v>
       </c>
       <c t="n" r="E11">
-        <v>73.33333333333333</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="F11">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="G11">
+        <v>43.333333333333336</v>
+      </c>
+      <c t="n" r="H11">
         <v>46.666666666666664</v>
       </c>
-      <c t="n" r="H11">
-        <v>70.0</v>
-      </c>
       <c t="n" r="I11">
-        <v>60.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="J11">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="K11">
-        <v>76.66666666666667</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="L11">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c t="n" r="M11">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c t="n" r="N11">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c t="n" r="O11">
+        <v>36.666666666666664</v>
+      </c>
+      <c t="n" r="P11">
+        <v>30.0</v>
+      </c>
+      <c t="n" r="Q11">
         <v>46.666666666666664</v>
       </c>
-      <c t="n" r="P11">
+      <c t="n" r="R11">
+        <v>30.0</v>
+      </c>
+      <c t="n" r="S11">
+        <v>23.333333333333332</v>
+      </c>
+      <c t="n" r="T11">
         <v>40.0</v>
-      </c>
-      <c t="n" r="Q11">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="R11">
-        <v>40.0</v>
-      </c>
-      <c t="n" r="S11">
-        <v>36.666666666666664</v>
-      </c>
-      <c t="n" r="T11">
-        <v>46.666666666666664</v>
       </c>
     </row>
     <row spans="1:20" r="12">
       <c t="s" r="A12">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c t="s" r="B12">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c t="n" r="C12">
-        <v>56.666666666666664</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="D12">
-        <v>53.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="E12">
-        <v>60.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="F12">
-        <v>56.666666666666664</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="G12">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="H12">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="I12">
         <v>46.666666666666664</v>
       </c>
-      <c t="n" r="H12">
+      <c t="n" r="J12">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="K12">
+        <v>70.0</v>
+      </c>
+      <c t="n" r="L12">
+        <v>47</v>
+      </c>
+      <c t="n" r="M12">
+        <v>92</v>
+      </c>
+      <c t="n" r="N12">
+        <v>47</v>
+      </c>
+      <c t="n" r="O12">
+        <v>43.333333333333336</v>
+      </c>
+      <c t="n" r="P12">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="Q12">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="R12">
+        <v>33.33333333333333</v>
+      </c>
+      <c t="n" r="S12">
         <v>50.0</v>
       </c>
-      <c t="n" r="I12">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="J12">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="K12">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="L12">
-        <v>48</v>
-      </c>
-      <c t="n" r="M12">
-        <v>94</v>
-      </c>
-      <c t="n" r="N12">
-        <v>48</v>
-      </c>
-      <c t="n" r="O12">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="P12">
-        <v>36.666666666666664</v>
-      </c>
-      <c t="n" r="Q12">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="R12">
-        <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="S12">
-        <v>30.0</v>
-      </c>
       <c t="n" r="T12">
-        <v>50.0</v>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row spans="1:20" r="13">
       <c t="s" r="A13">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c t="s" r="B13">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c t="n" r="C13">
-        <v>60.0</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="D13">
-        <v>60.0</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="E13">
-        <v>55.55555555555556</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="F13">
-        <v>60.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="G13">
-        <v>53.333333333333336</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="H13">
-        <v>44.44444444444444</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="I13">
-        <v>63.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="J13">
-        <v>66.66666666666666</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="K13">
-        <v>72.22222222222221</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="L13">
+        <v>46</v>
+      </c>
+      <c t="n" r="M13">
+        <v>91</v>
+      </c>
+      <c t="n" r="N13">
         <v>47</v>
       </c>
-      <c t="n" r="M13">
-        <v>65</v>
-      </c>
-      <c t="n" r="N13">
-        <v>18</v>
-      </c>
       <c t="n" r="O13">
-        <v>46.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="P13">
-        <v>53.333333333333336</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="Q13">
-        <v>66.66666666666666</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="R13">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="S13">
         <v>36.666666666666664</v>
       </c>
-      <c t="n" r="S13">
-        <v>46.666666666666664</v>
-      </c>
       <c t="n" r="T13">
-        <v>61.111111111111114</v>
+        <v>50.0</v>
       </c>
     </row>
     <row spans="1:20" r="14">
       <c t="s" r="A14">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c t="s" r="B14">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c t="n" r="C14">
-        <v>63.33333333333333</v>
+        <v>55.55555555555556</v>
       </c>
       <c t="n" r="D14">
-        <v>60.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="E14">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="F14">
         <v>50.0</v>
       </c>
-      <c t="n" r="F14">
-        <v>56.666666666666664</v>
-      </c>
       <c t="n" r="G14">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="H14">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="I14">
+        <v>55.55555555555556</v>
+      </c>
+      <c t="n" r="J14">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="K14">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="L14">
+        <v>18</v>
+      </c>
+      <c t="n" r="M14">
+        <v>63</v>
+      </c>
+      <c t="n" r="N14">
+        <v>46</v>
+      </c>
+      <c t="n" r="O14">
+        <v>44.44444444444444</v>
+      </c>
+      <c t="n" r="P14">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="Q14">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="R14">
+        <v>27.77777777777778</v>
+      </c>
+      <c t="n" r="S14">
+        <v>43.333333333333336</v>
+      </c>
+      <c t="n" r="T14">
         <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="I14">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="J14">
-        <v>60.0</v>
-      </c>
-      <c t="n" r="K14">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="L14">
-        <v>48</v>
-      </c>
-      <c t="n" r="M14">
-        <v>95</v>
-      </c>
-      <c t="n" r="N14">
-        <v>48</v>
-      </c>
-      <c t="n" r="O14">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="P14">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="Q14">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="R14">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="S14">
-        <v>40.0</v>
-      </c>
-      <c t="n" r="T14">
-        <v>43.333333333333336</v>
       </c>
     </row>
     <row spans="1:20" r="15">
       <c t="s" r="A15">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c t="s" r="B15">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c t="n" r="C15">
-        <v>73.33333333333333</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="D15">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="E15">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="F15">
+        <v>43.333333333333336</v>
+      </c>
+      <c t="n" r="G15">
+        <v>46.666666666666664</v>
+      </c>
+      <c t="n" r="H15">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="I15">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="J15">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="K15">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="L15">
+        <v>45</v>
+      </c>
+      <c t="n" r="M15">
+        <v>86</v>
+      </c>
+      <c t="n" r="N15">
+        <v>44</v>
+      </c>
+      <c t="n" r="O15">
+        <v>43.333333333333336</v>
+      </c>
+      <c t="n" r="P15">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="Q15">
         <v>70.0</v>
       </c>
-      <c t="n" r="E15">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="F15">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="G15">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="H15">
-        <v>60.0</v>
-      </c>
-      <c t="n" r="I15">
-        <v>76.66666666666667</v>
-      </c>
-      <c t="n" r="J15">
-        <v>73.33333333333333</v>
-      </c>
-      <c t="n" r="K15">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="L15">
-        <v>46</v>
-      </c>
-      <c t="n" r="M15">
-        <v>92</v>
-      </c>
-      <c t="n" r="N15">
-        <v>47</v>
-      </c>
-      <c t="n" r="O15">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="P15">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="Q15">
-        <v>60.0</v>
-      </c>
       <c t="n" r="R15">
-        <v>63.33333333333333</v>
+        <v>30.0</v>
       </c>
       <c t="n" r="S15">
-        <v>56.666666666666664</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="T15">
-        <v>50.0</v>
+        <v>46.666666666666664</v>
       </c>
     </row>
     <row spans="1:20" r="16">
       <c t="s" r="A16">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c t="s" r="B16">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c t="n" r="C16">
-        <v>56.666666666666664</v>
+        <v>86.66666666666667</v>
       </c>
       <c t="n" r="D16">
-        <v>56.666666666666664</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="E16">
-        <v>60.71428571428571</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="F16">
-        <v>43.333333333333336</v>
+        <v>83.33333333333334</v>
       </c>
       <c t="n" r="G16">
-        <v>46.666666666666664</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="H16">
-        <v>57.14285714285714</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="I16">
-        <v>60.0</v>
+        <v>86.66666666666667</v>
       </c>
       <c t="n" r="J16">
-        <v>63.33333333333333</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="K16">
-        <v>64.28571428571429</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="L16">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c t="n" r="M16">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c t="n" r="N16">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c t="n" r="O16">
-        <v>56.666666666666664</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="P16">
-        <v>56.666666666666664</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="Q16">
-        <v>60.71428571428571</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="R16">
-        <v>36.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="S16">
-        <v>40.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="T16">
-        <v>46.42857142857143</v>
+        <v>63.33333333333333</v>
       </c>
     </row>
     <row spans="1:20" r="17">
       <c t="s" r="A17">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c t="s" r="B17">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c t="n" r="C17">
-        <v>73.33333333333333</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="D17">
-        <v>73.33333333333333</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="E17">
-        <v>63.33333333333333</v>
+        <v>57.14285714285714</v>
       </c>
       <c t="n" r="F17">
-        <v>63.33333333333333</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="G17">
-        <v>66.66666666666666</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="H17">
-        <v>53.333333333333336</v>
+        <v>53.57142857142857</v>
       </c>
       <c t="n" r="I17">
-        <v>80.0</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="J17">
-        <v>76.66666666666667</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="K17">
-        <v>63.33333333333333</v>
+        <v>67.85714285714286</v>
       </c>
       <c t="n" r="L17">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c t="n" r="M17">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c t="n" r="N17">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c t="n" r="O17">
-        <v>63.33333333333333</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="P17">
-        <v>56.666666666666664</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="Q17">
-        <v>66.66666666666666</v>
+        <v>53.57142857142857</v>
       </c>
       <c t="n" r="R17">
-        <v>46.666666666666664</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="S17">
-        <v>46.666666666666664</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="T17">
-        <v>56.666666666666664</v>
+        <v>42.857142857142854</v>
       </c>
     </row>
     <row spans="1:20" r="18">
       <c t="s" r="A18">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c t="s" r="B18">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c t="n" r="C18">
-        <v>66.66666666666666</v>
+        <v>55.55555555555556</v>
       </c>
       <c t="n" r="D18">
-        <v>56.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="E18">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="F18">
+        <v>55.55555555555556</v>
+      </c>
+      <c t="n" r="G18">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="H18">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="I18">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="J18">
+        <v>70.0</v>
+      </c>
+      <c t="n" r="K18">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="L18">
+        <v>18</v>
+      </c>
+      <c t="n" r="M18">
+        <v>62</v>
+      </c>
+      <c t="n" r="N18">
+        <v>45</v>
+      </c>
+      <c t="n" r="O18">
+        <v>50.0</v>
+      </c>
+      <c t="n" r="P18">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="Q18">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="R18">
         <v>44.44444444444444</v>
       </c>
-      <c t="n" r="F18">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="G18">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="H18">
-        <v>38.88888888888889</v>
-      </c>
-      <c t="n" r="I18">
-        <v>73.33333333333333</v>
-      </c>
-      <c t="n" r="J18">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="K18">
-        <v>55.55555555555556</v>
-      </c>
-      <c t="n" r="L18">
-        <v>48</v>
-      </c>
-      <c t="n" r="M18">
-        <v>66</v>
-      </c>
-      <c t="n" r="N18">
-        <v>18</v>
-      </c>
-      <c t="n" r="O18">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="P18">
-        <v>60.0</v>
-      </c>
-      <c t="n" r="Q18">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="R18">
-        <v>36.666666666666664</v>
-      </c>
       <c t="n" r="S18">
-        <v>53.333333333333336</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="T18">
-        <v>66.66666666666666</v>
+        <v>40.0</v>
       </c>
     </row>
     <row spans="1:20" r="19">
       <c t="s" r="A19">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c t="s" r="B19">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c t="n" r="C19">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="D19">
-        <v>50.0</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="E19">
-        <v>60.0</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="F19">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="G19">
         <v>46.666666666666664</v>
       </c>
       <c t="n" r="H19">
-        <v>56.666666666666664</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="I19">
-        <v>53.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="J19">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="K19">
-        <v>66.66666666666666</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="L19">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c t="n" r="M19">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c t="n" r="N19">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c t="n" r="O19">
-        <v>56.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="P19">
-        <v>43.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="Q19">
-        <v>40.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="R19">
-        <v>46.666666666666664</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="S19">
-        <v>36.666666666666664</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="T19">
-        <v>36.666666666666664</v>
+        <v>50.0</v>
       </c>
     </row>
     <row spans="1:20" r="20">
       <c t="s" r="A20">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c t="s" r="B20">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c t="n" r="C20">
-        <v>60.0</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="D20">
-        <v>73.33333333333333</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="E20">
-        <v>66.66666666666666</v>
+        <v>nan</v>
       </c>
       <c t="n" r="F20">
         <v>50.0</v>
       </c>
       <c t="n" r="G20">
-        <v>66.66666666666666</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="H20">
-        <v>66.66666666666666</v>
+        <v>nan</v>
       </c>
       <c t="n" r="I20">
-        <v>66.66666666666666</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="J20">
-        <v>76.66666666666667</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="K20">
-        <v>70.0</v>
+        <v>nan</v>
       </c>
       <c t="n" r="L20">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c t="n" r="M20">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c t="n" r="N20">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c t="n" r="O20">
         <v>63.33333333333333</v>
       </c>
       <c t="n" r="P20">
-        <v>80.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="Q20">
-        <v>80.0</v>
+        <v>nan</v>
       </c>
       <c t="n" r="R20">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="S20">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="T20">
-        <v>60.0</v>
+        <v>nan</v>
       </c>
     </row>
     <row spans="1:20" r="21">
       <c t="s" r="A21">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c t="s" r="B21">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c t="n" r="C21">
-        <v>53.333333333333336</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="D21">
-        <v>56.666666666666664</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="E21">
-        <v>63.33333333333333</v>
+        <v>72.22222222222221</v>
       </c>
       <c t="n" r="F21">
-        <v>46.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="G21">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="H21">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="I21">
+        <v>70.0</v>
+      </c>
+      <c t="n" r="J21">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="K21">
+        <v>72.22222222222221</v>
+      </c>
+      <c t="n" r="L21">
+        <v>44</v>
+      </c>
+      <c t="n" r="M21">
+        <v>61</v>
+      </c>
+      <c t="n" r="N21">
+        <v>18</v>
+      </c>
+      <c t="n" r="O21">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="P21">
         <v>50.0</v>
       </c>
-      <c t="n" r="H21">
-        <v>60.0</v>
-      </c>
-      <c t="n" r="I21">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="J21">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="K21">
-        <v>70.0</v>
-      </c>
-      <c t="n" r="L21">
-        <v>47</v>
-      </c>
-      <c t="n" r="M21">
-        <v>92</v>
-      </c>
-      <c t="n" r="N21">
-        <v>46</v>
-      </c>
-      <c t="n" r="O21">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="P21">
-        <v>73.33333333333333</v>
-      </c>
       <c t="n" r="Q21">
-        <v>80.0</v>
+        <v>38.88888888888889</v>
       </c>
       <c t="n" r="R21">
         <v>60.0</v>
       </c>
       <c t="n" r="S21">
-        <v>63.33333333333333</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="T21">
-        <v>66.66666666666666</v>
+        <v>27.77777777777778</v>
       </c>
     </row>
     <row spans="1:20" r="22">
       <c t="s" r="A22">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c t="s" r="B22">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c t="n" r="C22">
-        <v>60.0</v>
+        <v>51.85185185185185</v>
       </c>
       <c t="n" r="D22">
-        <v>53.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="E22">
-        <v>60.0</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="F22">
-        <v>53.333333333333336</v>
+        <v>48.148148148148145</v>
       </c>
       <c t="n" r="G22">
         <v>53.333333333333336</v>
       </c>
       <c t="n" r="H22">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="I22">
-        <v>63.33333333333333</v>
+        <v>59.25925925925925</v>
       </c>
       <c t="n" r="J22">
-        <v>53.333333333333336</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="K22">
-        <v>63.33333333333333</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="L22">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c t="n" r="M22">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c t="n" r="N22">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c t="n" r="O22">
+        <v>48.148148148148145</v>
+      </c>
+      <c t="n" r="P22">
         <v>76.66666666666667</v>
       </c>
-      <c t="n" r="P22">
-        <v>70.0</v>
-      </c>
       <c t="n" r="Q22">
-        <v>60.0</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="R22">
-        <v>63.33333333333333</v>
+        <v>40.74074074074074</v>
       </c>
       <c t="n" r="S22">
-        <v>50.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="T22">
-        <v>36.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
     </row>
     <row spans="1:20" r="23">
       <c t="s" r="A23">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c t="s" r="B23">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c t="n" r="C23">
-        <v>55.55555555555556</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="D23">
-        <v>66.66666666666666</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="E23">
-        <v>56.666666666666664</v>
+        <v>58.82352941176471</v>
       </c>
       <c t="n" r="F23">
-        <v>55.55555555555556</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="G23">
-        <v>63.33333333333333</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="H23">
-        <v>53.333333333333336</v>
+        <v>52.94117647058824</v>
       </c>
       <c t="n" r="I23">
-        <v>66.66666666666666</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="J23">
-        <v>73.33333333333333</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="K23">
-        <v>63.33333333333333</v>
+        <v>58.82352941176471</v>
       </c>
       <c t="n" r="L23">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c t="n" r="M23">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c t="n" r="N23">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c t="n" r="O23">
-        <v>50.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="P23">
-        <v>53.333333333333336</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="Q23">
-        <v>53.333333333333336</v>
+        <v>76.47058823529412</v>
       </c>
       <c t="n" r="R23">
-        <v>44.44444444444444</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="S23">
-        <v>46.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="T23">
-        <v>40.0</v>
+        <v>58.82352941176471</v>
       </c>
     </row>
     <row spans="1:20" r="24">
       <c t="s" r="A24">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c t="s" r="B24">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c t="n" r="C24">
-        <v>36.666666666666664</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="D24">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="E24">
-        <v>56.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="F24">
-        <v>36.666666666666664</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="G24">
-        <v>36.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="H24">
-        <v>53.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="I24">
-        <v>36.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="J24">
-        <v>43.333333333333336</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="K24">
-        <v>60.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="L24">
         <v>46</v>
       </c>
       <c t="n" r="M24">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c t="n" r="N24">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c t="n" r="O24">
+        <v>56.666666666666664</v>
+      </c>
+      <c t="n" r="P24">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="Q24">
+        <v>50.0</v>
+      </c>
+      <c t="n" r="R24">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="S24">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="T24">
         <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="P24">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="Q24">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="R24">
-        <v>36.666666666666664</v>
-      </c>
-      <c t="n" r="S24">
-        <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="T24">
-        <v>50.0</v>
       </c>
     </row>
     <row spans="1:20" r="25">
       <c t="s" r="A25">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c t="s" r="B25">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c t="n" r="C25">
-        <v>66.66666666666666</v>
+        <v>80.0</v>
       </c>
       <c t="n" r="D25">
-        <v>50.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="E25">
-        <v>43.333333333333336</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="F25">
-        <v>63.33333333333333</v>
+        <v>80.0</v>
       </c>
       <c t="n" r="G25">
-        <v>46.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="H25">
-        <v>40.0</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="I25">
-        <v>70.0</v>
+        <v>80.0</v>
       </c>
       <c t="n" r="J25">
-        <v>53.333333333333336</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="K25">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="L25">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c t="n" r="M25">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c t="n" r="N25">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c t="n" r="O25">
-        <v>66.66666666666666</v>
+        <v>76.66666666666667</v>
       </c>
       <c t="n" r="P25">
-        <v>60.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="Q25">
         <v>60.0</v>
@@ -2377,452 +2314,452 @@
         <v>60.0</v>
       </c>
       <c t="n" r="S25">
-        <v>40.0</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="T25">
-        <v>33.33333333333333</v>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row spans="1:20" r="26">
       <c t="s" r="A26">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c t="s" r="B26">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c t="n" r="C26">
-        <v>56.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="D26">
-        <v>63.33333333333333</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="E26">
-        <v>60.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="F26">
-        <v>46.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="G26">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="H26">
-        <v>53.333333333333336</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="I26">
-        <v>60.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="J26">
-        <v>66.66666666666666</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="K26">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="L26">
+        <v>48</v>
+      </c>
+      <c t="n" r="M26">
+        <v>91</v>
+      </c>
+      <c t="n" r="N26">
         <v>46</v>
       </c>
-      <c t="n" r="M26">
-        <v>89</v>
-      </c>
-      <c t="n" r="N26">
-        <v>45</v>
-      </c>
       <c t="n" r="O26">
-        <v>63.33333333333333</v>
+        <v>80.0</v>
       </c>
       <c t="n" r="P26">
-        <v>63.33333333333333</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="Q26">
-        <v>60.0</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="R26">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="S26">
-        <v>36.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="T26">
-        <v>53.333333333333336</v>
+        <v>50.0</v>
       </c>
     </row>
     <row spans="1:20" r="27">
       <c t="s" r="A27">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c t="s" r="B27">
+        <v>69</v>
+      </c>
+      <c t="n" r="C27">
+        <v>nan</v>
+      </c>
+      <c t="n" r="D27">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="E27">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="F27">
+        <v>nan</v>
+      </c>
+      <c t="n" r="G27">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="H27">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="I27">
+        <v>nan</v>
+      </c>
+      <c t="n" r="J27">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="K27">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="L27">
+        <v>0</v>
+      </c>
+      <c t="n" r="M27">
         <v>45</v>
       </c>
-      <c t="n" r="C27">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="D27">
-        <v>60.0</v>
-      </c>
-      <c t="n" r="E27">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="F27">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="G27">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="H27">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="I27">
-        <v>70.0</v>
-      </c>
-      <c t="n" r="J27">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="K27">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="L27">
-        <v>44</v>
-      </c>
-      <c t="n" r="M27">
-        <v>86</v>
-      </c>
       <c t="n" r="N27">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c t="n" r="O27">
-        <v>66.66666666666666</v>
+        <v>nan</v>
       </c>
       <c t="n" r="P27">
-        <v>70.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="Q27">
-        <v>73.33333333333333</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="R27">
-        <v>43.333333333333336</v>
+        <v>nan</v>
       </c>
       <c t="n" r="S27">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="T27">
-        <v>63.33333333333333</v>
+        <v>56.666666666666664</v>
       </c>
     </row>
     <row spans="1:20" r="28">
       <c t="s" r="A28">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c t="s" r="B28">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c t="n" r="C28">
-        <v>70.0</v>
+        <v>55.55555555555556</v>
       </c>
       <c t="n" r="D28">
-        <v>80.0</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="E28">
-        <v>60.0</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="F28">
-        <v>66.66666666666666</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="G28">
-        <v>80.0</v>
+        <v>33.33333333333333</v>
       </c>
       <c t="n" r="H28">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="I28">
-        <v>73.33333333333333</v>
+        <v>55.55555555555556</v>
       </c>
       <c t="n" r="J28">
-        <v>86.66666666666667</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="K28">
-        <v>66.66666666666666</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="L28">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c t="n" r="M28">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c t="n" r="N28">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c t="n" r="O28">
-        <v>56.666666666666664</v>
+        <v>44.44444444444444</v>
       </c>
       <c t="n" r="P28">
-        <v>56.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="Q28">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="R28">
-        <v>36.666666666666664</v>
+        <v>27.77777777777778</v>
       </c>
       <c t="n" r="S28">
-        <v>40.0</v>
+        <v>33.33333333333333</v>
       </c>
       <c t="n" r="T28">
-        <v>46.666666666666664</v>
+        <v>33.33333333333333</v>
       </c>
     </row>
     <row spans="1:20" r="29">
       <c t="s" r="A29">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c t="s" r="B29">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c t="n" r="C29">
-        <v>43.333333333333336</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="D29">
-        <v>53.333333333333336</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="E29">
-        <v>72.22222222222221</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="F29">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="G29">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="H29">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="I29">
+        <v>73.33333333333333</v>
+      </c>
+      <c t="n" r="J29">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="K29">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="L29">
+        <v>45</v>
+      </c>
+      <c t="n" r="M29">
+        <v>88</v>
+      </c>
+      <c t="n" r="N29">
+        <v>46</v>
+      </c>
+      <c t="n" r="O29">
+        <v>80.0</v>
+      </c>
+      <c t="n" r="P29">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="Q29">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="R29">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="S29">
+        <v>46.666666666666664</v>
+      </c>
+      <c t="n" r="T29">
         <v>40.0</v>
-      </c>
-      <c t="n" r="G29">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="H29">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="I29">
-        <v>46.666666666666664</v>
-      </c>
-      <c t="n" r="J29">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="K29">
-        <v>72.22222222222221</v>
-      </c>
-      <c t="n" r="L29">
-        <v>47</v>
-      </c>
-      <c t="n" r="M29">
-        <v>65</v>
-      </c>
-      <c t="n" r="N29">
-        <v>18</v>
-      </c>
-      <c t="n" r="O29">
-        <v>43.333333333333336</v>
-      </c>
-      <c t="n" r="P29">
-        <v>43.333333333333336</v>
-      </c>
-      <c t="n" r="Q29">
-        <v>38.88888888888889</v>
-      </c>
-      <c t="n" r="R29">
-        <v>33.33333333333333</v>
-      </c>
-      <c t="n" r="S29">
-        <v>30.0</v>
-      </c>
-      <c t="n" r="T29">
-        <v>27.77777777777778</v>
       </c>
     </row>
     <row spans="1:20" r="30">
       <c t="s" r="A30">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c t="s" r="B30">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c t="n" r="C30">
-        <v>56.666666666666664</v>
+        <v>52.63157894736842</v>
       </c>
       <c t="n" r="D30">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="E30">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="F30">
+        <v>52.63157894736842</v>
+      </c>
+      <c t="n" r="G30">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="H30">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="I30">
+        <v>52.63157894736842</v>
+      </c>
+      <c t="n" r="J30">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="K30">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="L30">
+        <v>19</v>
+      </c>
+      <c t="n" r="M30">
+        <v>62</v>
+      </c>
+      <c t="n" r="N30">
+        <v>44</v>
+      </c>
+      <c t="n" r="O30">
+        <v>52.63157894736842</v>
+      </c>
+      <c t="n" r="P30">
+        <v>50.0</v>
+      </c>
+      <c t="n" r="Q30">
+        <v>46.666666666666664</v>
+      </c>
+      <c t="n" r="R30">
+        <v>42.10526315789473</v>
+      </c>
+      <c t="n" r="S30">
         <v>43.333333333333336</v>
       </c>
-      <c t="n" r="E30">
-        <v>51.85185185185185</v>
-      </c>
-      <c t="n" r="F30">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="G30">
-        <v>43.333333333333336</v>
-      </c>
-      <c t="n" r="H30">
-        <v>48.148148148148145</v>
-      </c>
-      <c t="n" r="I30">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="J30">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="K30">
-        <v>55.55555555555556</v>
-      </c>
-      <c t="n" r="L30">
-        <v>46</v>
-      </c>
-      <c t="n" r="M30">
-        <v>72</v>
-      </c>
-      <c t="n" r="N30">
-        <v>27</v>
-      </c>
-      <c t="n" r="O30">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="P30">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="Q30">
-        <v>62.96296296296296</v>
-      </c>
-      <c t="n" r="R30">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="S30">
-        <v>46.666666666666664</v>
-      </c>
       <c t="n" r="T30">
-        <v>48.148148148148145</v>
+        <v>40.0</v>
       </c>
     </row>
     <row spans="1:20" r="31">
       <c t="s" r="A31">
+        <v>29</v>
+      </c>
+      <c t="s" r="B31">
+        <v>55</v>
+      </c>
+      <c t="n" r="C31">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="D31">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="E31">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="F31">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="G31">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="H31">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="I31">
+        <v>63.33333333333333</v>
+      </c>
+      <c t="n" r="J31">
+        <v>60.0</v>
+      </c>
+      <c t="n" r="K31">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="L31">
         <v>43</v>
       </c>
-      <c t="s" r="B31">
-        <v>68</v>
-      </c>
-      <c t="n" r="C31">
-        <v>80.0</v>
-      </c>
-      <c t="n" r="D31">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="E31">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="F31">
-        <v>80.0</v>
-      </c>
-      <c t="n" r="G31">
-        <v>63.33333333333333</v>
-      </c>
-      <c t="n" r="H31">
-        <v>50.0</v>
-      </c>
-      <c t="n" r="I31">
-        <v>80.0</v>
-      </c>
-      <c t="n" r="J31">
-        <v>70.0</v>
-      </c>
-      <c t="n" r="K31">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="L31">
+      <c t="n" r="M31">
+        <v>87</v>
+      </c>
+      <c t="n" r="N31">
         <v>46</v>
-      </c>
-      <c t="n" r="M31">
-        <v>81</v>
-      </c>
-      <c t="n" r="N31">
-        <v>36</v>
       </c>
       <c t="n" r="O31">
         <v>76.66666666666667</v>
       </c>
       <c t="n" r="P31">
-        <v>83.33333333333334</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="Q31">
-        <v>73.33333333333333</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="R31">
-        <v>60.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="S31">
-        <v>73.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="T31">
-        <v>63.33333333333333</v>
+        <v>46.666666666666664</v>
       </c>
     </row>
     <row spans="1:20" r="32">
       <c t="s" r="A32">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c t="s" r="B32">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c t="n" r="C32">
-        <v>70.0</v>
+        <v>80.0</v>
       </c>
       <c t="n" r="D32">
-        <v>60.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="E32">
-        <v>63.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="F32">
-        <v>66.66666666666666</v>
+        <v>80.0</v>
       </c>
       <c t="n" r="G32">
-        <v>56.666666666666664</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="H32">
-        <v>60.0</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="I32">
-        <v>73.33333333333333</v>
+        <v>80.0</v>
       </c>
       <c t="n" r="J32">
-        <v>63.33333333333333</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="K32">
-        <v>63.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="L32">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c t="n" r="M32">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c t="n" r="N32">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c t="n" r="O32">
-        <v>50.0</v>
+        <v>76.66666666666667</v>
       </c>
       <c t="n" r="P32">
-        <v>63.33333333333333</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="Q32">
-        <v>73.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="R32">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="S32">
         <v>53.333333333333336</v>
       </c>
       <c t="n" r="T32">
-        <v>66.66666666666666</v>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row spans="1:20" r="33">
       <c t="s" r="A33">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c t="s" r="B33">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c t="n" r="C33">
         <v>56.666666666666664</v>
@@ -2843,7 +2780,7 @@
         <v>73.33333333333333</v>
       </c>
       <c t="n" r="I33">
-        <v>63.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="J33">
         <v>66.66666666666666</v>
@@ -2852,28 +2789,28 @@
         <v>80.0</v>
       </c>
       <c t="n" r="L33">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c t="n" r="M33">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c t="n" r="N33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c t="n" r="O33">
-        <v>50.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="P33">
-        <v>60.0</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="Q33">
         <v>56.666666666666664</v>
       </c>
       <c t="n" r="R33">
-        <v>30.0</v>
+        <v>26.666666666666668</v>
       </c>
       <c t="n" r="S33">
-        <v>36.666666666666664</v>
+        <v>33.33333333333333</v>
       </c>
       <c t="n" r="T33">
         <v>40.0</v>
@@ -2881,28 +2818,28 @@
     </row>
     <row spans="1:20" r="34">
       <c t="s" r="A34">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c t="s" r="B34">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c t="n" r="C34">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="D34">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="E34">
-        <v>56.25</v>
+        <v>52.94117647058824</v>
       </c>
       <c t="n" r="F34">
-        <v>43.333333333333336</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="G34">
         <v>46.666666666666664</v>
       </c>
       <c t="n" r="H34">
-        <v>50.0</v>
+        <v>47.05882352941176</v>
       </c>
       <c t="n" r="I34">
         <v>60.0</v>
@@ -2911,57 +2848,57 @@
         <v>63.33333333333333</v>
       </c>
       <c t="n" r="K34">
-        <v>62.5</v>
+        <v>64.70588235294117</v>
       </c>
       <c t="n" r="L34">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c t="n" r="M34">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c t="n" r="N34">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c t="n" r="O34">
-        <v>66.66666666666666</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="P34">
         <v>50.0</v>
       </c>
       <c t="n" r="Q34">
-        <v>31.25</v>
+        <v>29.411764705882355</v>
       </c>
       <c t="n" r="R34">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="S34">
         <v>40.0</v>
       </c>
       <c t="n" r="T34">
-        <v>25.0</v>
+        <v>23.52941176470588</v>
       </c>
     </row>
     <row spans="1:20" r="35">
       <c t="s" r="A35">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c t="s" r="B35">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c t="n" r="C35">
-        <v>63.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="D35">
-        <v>70.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="E35">
         <v>60.0</v>
       </c>
       <c t="n" r="F35">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="G35">
-        <v>70.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="H35">
         <v>60.0</v>
@@ -2973,104 +2910,104 @@
         <v>70.0</v>
       </c>
       <c t="n" r="K35">
-        <v>60.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="L35">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c t="n" r="M35">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c t="n" r="N35">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c t="n" r="O35">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="P35">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="Q35">
-        <v>53.333333333333336</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="R35">
-        <v>33.33333333333333</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="S35">
-        <v>33.33333333333333</v>
+        <v>36.666666666666664</v>
       </c>
       <c t="n" r="T35">
-        <v>36.666666666666664</v>
+        <v>40.0</v>
       </c>
     </row>
     <row spans="1:20" r="36">
       <c t="s" r="A36">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c t="s" r="B36">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c t="n" r="C36">
         <v>80.0</v>
       </c>
       <c t="n" r="D36">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="E36">
+        <v>50.0</v>
+      </c>
+      <c t="n" r="F36">
+        <v>66.66666666666666</v>
+      </c>
+      <c t="n" r="G36">
+        <v>53.333333333333336</v>
+      </c>
+      <c t="n" r="H36">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="I36">
+        <v>80.0</v>
+      </c>
+      <c t="n" r="J36">
         <v>70.0</v>
       </c>
-      <c t="n" r="E36">
-        <v>53.333333333333336</v>
-      </c>
-      <c t="n" r="F36">
-        <v>66.66666666666666</v>
-      </c>
-      <c t="n" r="G36">
-        <v>56.666666666666664</v>
-      </c>
-      <c t="n" r="H36">
-        <v>43.333333333333336</v>
-      </c>
-      <c t="n" r="I36">
-        <v>83.33333333333334</v>
-      </c>
-      <c t="n" r="J36">
-        <v>73.33333333333333</v>
-      </c>
       <c t="n" r="K36">
-        <v>60.0</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="L36">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c t="n" r="M36">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c t="n" r="N36">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c t="n" r="O36">
         <v>40.0</v>
       </c>
       <c t="n" r="P36">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="Q36">
-        <v>50.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="R36">
         <v>33.33333333333333</v>
       </c>
       <c t="n" r="S36">
-        <v>43.333333333333336</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="T36">
-        <v>33.33333333333333</v>
+        <v>30.0</v>
       </c>
     </row>
     <row spans="1:20" r="37">
       <c t="s" r="A37">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c t="s" r="B37">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c t="n" r="C37">
         <v>63.33333333333333</v>
@@ -3079,16 +3016,16 @@
         <v>63.33333333333333</v>
       </c>
       <c t="n" r="E37">
-        <v>63.33333333333333</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="F37">
         <v>63.33333333333333</v>
       </c>
       <c t="n" r="G37">
-        <v>56.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="H37">
-        <v>56.666666666666664</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="I37">
         <v>70.0</v>
@@ -3097,25 +3034,25 @@
         <v>66.66666666666666</v>
       </c>
       <c t="n" r="K37">
-        <v>63.33333333333333</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="L37">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c t="n" r="M37">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c t="n" r="N37">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c t="n" r="O37">
-        <v>40.0</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="P37">
         <v>43.333333333333336</v>
       </c>
       <c t="n" r="Q37">
-        <v>46.666666666666664</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="R37">
         <v>30.0</v>
@@ -3129,46 +3066,46 @@
     </row>
     <row spans="1:20" r="38">
       <c t="s" r="A38">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c t="s" r="B38">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c t="n" r="C38">
         <v>66.66666666666666</v>
       </c>
       <c t="n" r="D38">
-        <v>66.66666666666666</v>
+        <v>70.0</v>
       </c>
       <c t="n" r="E38">
         <v>70.0</v>
       </c>
       <c t="n" r="F38">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="G38">
         <v>56.666666666666664</v>
       </c>
       <c t="n" r="H38">
-        <v>60.0</v>
+        <v>56.666666666666664</v>
       </c>
       <c t="n" r="I38">
         <v>70.0</v>
       </c>
       <c t="n" r="J38">
-        <v>70.0</v>
+        <v>73.33333333333333</v>
       </c>
       <c t="n" r="K38">
         <v>70.0</v>
       </c>
       <c t="n" r="L38">
+        <v>42</v>
+      </c>
+      <c t="n" r="M38">
+        <v>81</v>
+      </c>
+      <c t="n" r="N38">
         <v>41</v>
-      </c>
-      <c t="n" r="M38">
-        <v>80</v>
-      </c>
-      <c t="n" r="N38">
-        <v>40</v>
       </c>
       <c t="n" r="O38">
         <v>56.666666666666664</v>
@@ -3191,111 +3128,111 @@
     </row>
     <row spans="1:20" r="39">
       <c t="s" r="A39">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c t="s" r="B39">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c t="n" r="C39">
-        <v>66.66666666666666</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="D39">
-        <v>63.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="E39">
         <v>56.666666666666664</v>
       </c>
       <c t="n" r="F39">
-        <v>56.666666666666664</v>
+        <v>53.333333333333336</v>
       </c>
       <c t="n" r="G39">
-        <v>46.666666666666664</v>
+        <v>43.333333333333336</v>
       </c>
       <c t="n" r="H39">
         <v>50.0</v>
       </c>
       <c t="n" r="I39">
-        <v>70.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="J39">
-        <v>70.0</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="K39">
         <v>63.33333333333333</v>
       </c>
       <c t="n" r="L39">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c t="n" r="M39">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c t="n" r="N39">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c t="n" r="O39">
         <v>56.666666666666664</v>
       </c>
       <c t="n" r="P39">
-        <v>63.33333333333333</v>
+        <v>60.0</v>
       </c>
       <c t="n" r="Q39">
-        <v>50.0</v>
+        <v>46.666666666666664</v>
       </c>
       <c t="n" r="R39">
         <v>40.0</v>
       </c>
       <c t="n" r="S39">
-        <v>43.333333333333336</v>
+        <v>40.0</v>
       </c>
       <c t="n" r="T39">
-        <v>26.666666666666668</v>
+        <v>23.333333333333332</v>
       </c>
     </row>
     <row spans="1:20" r="40">
       <c t="s" r="A40">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c t="s" r="B40">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c t="n" r="C40">
-        <v>60.0</v>
+        <v>62.5</v>
       </c>
       <c t="n" r="D40">
         <v>63.33333333333333</v>
       </c>
       <c t="n" r="E40">
-        <v>60.0</v>
+        <v>63.33333333333333</v>
       </c>
       <c t="n" r="F40">
-        <v>53.333333333333336</v>
+        <v>56.25</v>
       </c>
       <c t="n" r="G40">
         <v>50.0</v>
       </c>
       <c t="n" r="H40">
-        <v>46.666666666666664</v>
+        <v>50.0</v>
       </c>
       <c t="n" r="I40">
-        <v>60.0</v>
+        <v>62.5</v>
       </c>
       <c t="n" r="J40">
         <v>63.33333333333333</v>
       </c>
       <c t="n" r="K40">
-        <v>63.33333333333333</v>
+        <v>66.66666666666666</v>
       </c>
       <c t="n" r="L40">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c t="n" r="M40">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c t="n" r="N40">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c t="n" r="O40">
-        <v>40.0</v>
+        <v>37.5</v>
       </c>
       <c t="n" r="P40">
         <v>33.33333333333333</v>
@@ -3304,7 +3241,7 @@
         <v>36.666666666666664</v>
       </c>
       <c t="n" r="R40">
-        <v>33.33333333333333</v>
+        <v>31.25</v>
       </c>
       <c t="n" r="S40">
         <v>30.0</v>
@@ -4547,10 +4484,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:G40">
-    <cfRule priority="2" dxfId="2" type="cellIs" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>30</formula>
     </cfRule>
-    <cfRule priority="1" dxfId="1" type="cellIs" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>70</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>